<commit_message>
fix(import): Update scenario and schemas according to client needs.
</commit_message>
<xml_diff>
--- a/src/import/Nov_21_2016/CompetitorVariant.xlsx
+++ b/src/import/Nov_21_2016/CompetitorVariant.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -336,6 +337,9 @@
   </si>
   <si>
     <t>مكرونة مقطعة</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PIECES &amp; STEMS 2</t>
   </si>
 </sst>
 </file>
@@ -476,17 +480,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -772,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1301,7 +1295,7 @@
         <v>44</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>86</v>
@@ -1410,32 +1404,8 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B45">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Variant!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B42</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Category!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D42 D44:D45</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Variant!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2 C32 C4 C6:C30 C34:C42</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>